<commit_message>
Cleaned and removed (moved into the old files folder)
</commit_message>
<xml_diff>
--- a/output/final_merged_summary_replace_TRUE.xlsx
+++ b/output/final_merged_summary_replace_TRUE.xlsx
@@ -437,7 +437,7 @@
         <v>8.484484484484485</v>
       </c>
       <c r="I2">
-        <v>0.05727950172394617</v>
+        <v>0.05727950172394616</v>
       </c>
       <c r="J2">
         <v>0.5155155155155156</v>
@@ -471,7 +471,7 @@
         <v>8.933933933933934</v>
       </c>
       <c r="I3">
-        <v>0.007340674007340669</v>
+        <v>0.007340674007340673</v>
       </c>
       <c r="J3">
         <v>0.06606606606606606</v>
@@ -913,7 +913,7 @@
         <v>3.158158158158158</v>
       </c>
       <c r="I16">
-        <v>0.6447856586745476</v>
+        <v>0.6447856586745475</v>
       </c>
       <c r="J16">
         <v>5.735735735735735</v>
@@ -947,7 +947,7 @@
         <v>1.107305936073059</v>
       </c>
       <c r="I17">
-        <v>0.4720414764079147</v>
+        <v>0.4720414764079148</v>
       </c>
       <c r="J17">
         <v>0.9554794520547946</v>
@@ -1049,7 +1049,7 @@
         <v>8.425425425425425</v>
       </c>
       <c r="I20">
-        <v>0.06384161939717499</v>
+        <v>0.06384161939717495</v>
       </c>
       <c r="J20">
         <v>0.5745745745745746</v>
@@ -1151,7 +1151,7 @@
         <v>7.93993993993994</v>
       </c>
       <c r="I23">
-        <v>0.1177844511177845</v>
+        <v>0.1177844511177844</v>
       </c>
       <c r="J23">
         <v>1.06006006006006</v>
@@ -1185,7 +1185,7 @@
         <v>8.953953953953954</v>
       </c>
       <c r="I24">
-        <v>0.005116227338449558</v>
+        <v>0.00511622733844956</v>
       </c>
       <c r="J24">
         <v>0.04604604604604605</v>
@@ -1287,7 +1287,7 @@
         <v>8.686686686686686</v>
       </c>
       <c r="I27">
-        <v>0.03481259036814591</v>
+        <v>0.03481259036814592</v>
       </c>
       <c r="J27">
         <v>0.3133133133133133</v>
@@ -1729,7 +1729,7 @@
         <v>7.064064064064064</v>
       </c>
       <c r="I40">
-        <v>0.2151039928817706</v>
+        <v>0.2151039928817707</v>
       </c>
       <c r="J40">
         <v>1.935935935935936</v>
@@ -1763,7 +1763,7 @@
         <v>8.961961961961961</v>
       </c>
       <c r="I41">
-        <v>0.004226448670893118</v>
+        <v>0.004226448670893115</v>
       </c>
       <c r="J41">
         <v>0.03803803803803804</v>
@@ -1865,7 +1865,7 @@
         <v>8.983983983983984</v>
       </c>
       <c r="I44">
-        <v>0.001779557335112887</v>
+        <v>0.001779557335112891</v>
       </c>
       <c r="J44">
         <v>0.01601601601601602</v>
@@ -2035,7 +2035,7 @@
         <v>8.916916916916916</v>
       </c>
       <c r="I49">
-        <v>0.009231453675898121</v>
+        <v>0.009231453675898119</v>
       </c>
       <c r="J49">
         <v>0.08308308308308308</v>
@@ -2137,7 +2137,7 @@
         <v>8.985985985985986</v>
       </c>
       <c r="I52">
-        <v>0.001557112668223778</v>
+        <v>0.001557112668223779</v>
       </c>
       <c r="J52">
         <v>0.01401401401401401</v>
@@ -2171,7 +2171,7 @@
         <v>8.33033033033033</v>
       </c>
       <c r="I53">
-        <v>0.07440774107440776</v>
+        <v>0.07440774107440774</v>
       </c>
       <c r="J53">
         <v>0.6696696696696697</v>
@@ -2239,7 +2239,7 @@
         <v>8.98998998998999</v>
       </c>
       <c r="I55">
-        <v>0.00111222333444556</v>
+        <v>0.001112223334445557</v>
       </c>
       <c r="J55">
         <v>0.01001001001001001</v>
@@ -2375,7 +2375,7 @@
         <v>0.9479479479479479</v>
       </c>
       <c r="I59">
-        <v>0.873137423137423</v>
+        <v>0.8731374231374232</v>
       </c>
       <c r="J59">
         <v>6.49049049049049</v>
@@ -2545,7 +2545,7 @@
         <v>0.9419419419419419</v>
       </c>
       <c r="I64">
-        <v>0.8867295867295868</v>
+        <v>0.8867295867295867</v>
       </c>
       <c r="J64">
         <v>7.374374374374375</v>
@@ -2953,7 +2953,7 @@
         <v>1.764408493427705</v>
       </c>
       <c r="I76">
-        <v>0.5251336125956956</v>
+        <v>0.5251336125956955</v>
       </c>
       <c r="J76">
         <v>1.977755308392315</v>
@@ -2987,7 +2987,7 @@
         <v>1.791791791791792</v>
       </c>
       <c r="I77">
-        <v>0.8003757725979949</v>
+        <v>0.8003757725979948</v>
       </c>
       <c r="J77">
         <v>7.177177177177177</v>
@@ -3361,7 +3361,7 @@
         <v>0.964964964964965</v>
       </c>
       <c r="I88">
-        <v>0.8767632712077156</v>
+        <v>0.8767632712077157</v>
       </c>
       <c r="J88">
         <v>6.811811811811812</v>
@@ -3463,7 +3463,7 @@
         <v>1.814814814814815</v>
       </c>
       <c r="I91">
-        <v>0.7816725455614345</v>
+        <v>0.7816725455614344</v>
       </c>
       <c r="J91">
         <v>6.506506506506507</v>
@@ -3633,7 +3633,7 @@
         <v>8.965965965965966</v>
       </c>
       <c r="I96">
-        <v>0.003781559337114903</v>
+        <v>0.003781559337114892</v>
       </c>
       <c r="J96">
         <v>0.03403403403403404</v>
@@ -3939,7 +3939,7 @@
         <v>4.76976976976977</v>
       </c>
       <c r="I105">
-        <v>0.4696641085529974</v>
+        <v>0.4696641085529975</v>
       </c>
       <c r="J105">
         <v>4.224224224224224</v>
@@ -4075,7 +4075,7 @@
         <v>0.9119119119119119</v>
       </c>
       <c r="I109">
-        <v>0.8579130718019607</v>
+        <v>0.8579130718019606</v>
       </c>
       <c r="J109">
         <v>5.541541541541542</v>
@@ -4143,7 +4143,7 @@
         <v>0.9459459459459459</v>
       </c>
       <c r="I111">
-        <v>0.8846191429524763</v>
+        <v>0.8846191429524762</v>
       </c>
       <c r="J111">
         <v>7.265265265265265</v>
@@ -4177,7 +4177,7 @@
         <v>0.95496417604913</v>
       </c>
       <c r="I112">
-        <v>0.6981905249305455</v>
+        <v>0.6981905249305453</v>
       </c>
       <c r="J112">
         <v>2.232343909928352</v>
@@ -4381,7 +4381,7 @@
         <v>7.781781781781782</v>
       </c>
       <c r="I118">
-        <v>0.1353575798020243</v>
+        <v>0.1353575798020242</v>
       </c>
       <c r="J118">
         <v>1.218218218218218</v>
@@ -4415,7 +4415,7 @@
         <v>8.94994994994995</v>
       </c>
       <c r="I119">
-        <v>0.005561116672227777</v>
+        <v>0.005561116672227783</v>
       </c>
       <c r="J119">
         <v>0.05005005005005005</v>
@@ -4517,7 +4517,7 @@
         <v>2.499491353001017</v>
       </c>
       <c r="I122">
-        <v>0.2082546141549194</v>
+        <v>0.2082546141549193</v>
       </c>
       <c r="J122">
         <v>0.671414038657172</v>
@@ -4585,7 +4585,7 @@
         <v>5.144144144144144</v>
       </c>
       <c r="I124">
-        <v>0.4263569124680236</v>
+        <v>0.4263569124680235</v>
       </c>
       <c r="J124">
         <v>3.825825825825826</v>
@@ -4687,7 +4687,7 @@
         <v>8.024024024024024</v>
       </c>
       <c r="I127">
-        <v>0.1084417751084417</v>
+        <v>0.1084417751084418</v>
       </c>
       <c r="J127">
         <v>0.975975975975976</v>
@@ -4755,7 +4755,7 @@
         <v>8.693693693693694</v>
       </c>
       <c r="I129">
-        <v>0.03403403403403406</v>
+        <v>0.03403403403403403</v>
       </c>
       <c r="J129">
         <v>0.3063063063063063</v>
@@ -4823,7 +4823,7 @@
         <v>4.721721721721722</v>
       </c>
       <c r="I131">
-        <v>0.4753642531420308</v>
+        <v>0.4753642531420309</v>
       </c>
       <c r="J131">
         <v>4.278278278278278</v>
@@ -4891,7 +4891,7 @@
         <v>8.975975975975976</v>
       </c>
       <c r="I133">
-        <v>0.002669336002669339</v>
+        <v>0.002669336002669336</v>
       </c>
       <c r="J133">
         <v>0.02402402402402402</v>
@@ -4959,7 +4959,7 @@
         <v>1.867303609341826</v>
       </c>
       <c r="I135">
-        <v>0.2971716712162571</v>
+        <v>0.2971716712162572</v>
       </c>
       <c r="J135">
         <v>0.8089171974522293</v>
@@ -5027,7 +5027,7 @@
         <v>8.998998998998999</v>
       </c>
       <c r="I137">
-        <v>0.000111222333444555</v>
+        <v>0.0001112223334445557</v>
       </c>
       <c r="J137">
         <v>0.001001001001001001</v>

</xml_diff>